<commit_message>
manejo de sql con dataframe
</commit_message>
<xml_diff>
--- a/archivo.xlsx
+++ b/archivo.xlsx
@@ -19,36 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>f</t>
+    <t>id</t>
   </si>
   <si>
-    <t>edad</t>
+    <t>multa</t>
   </si>
   <si>
-    <t>sexo</t>
+    <t>valores</t>
   </si>
   <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>actividad</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>soltero</t>
-  </si>
-  <si>
-    <t>casado</t>
-  </si>
-  <si>
-    <t>estudiante</t>
-  </si>
-  <si>
-    <t>ingeniero</t>
+    <t>dias</t>
   </si>
 </sst>
 </file>
@@ -390,80 +372,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>43</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>54</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>34</v>
+      </c>
+      <c r="D7">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
         <v>9</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prueba de visualizacion global de datos[C
</commit_message>
<xml_diff>
--- a/archivo.xlsx
+++ b/archivo.xlsx
@@ -19,25 +19,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>multa</t>
-  </si>
-  <si>
-    <t>valores</t>
-  </si>
-  <si>
-    <t>dias</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>IDENTIFICACION_DEUDOR</t>
+  </si>
+  <si>
+    <t>TIPO_IDENTIFICACION</t>
+  </si>
+  <si>
+    <t>NUMERO_CUENTA</t>
+  </si>
+  <si>
+    <t>ESTADO AXIS</t>
+  </si>
+  <si>
+    <t>ESTADO_CREDITO</t>
+  </si>
+  <si>
+    <t>SALDO</t>
+  </si>
+  <si>
+    <t>DIAS_MORA</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>CODIGO_CONDICION</t>
+  </si>
+  <si>
+    <t>PLACA_VEHICULO</t>
+  </si>
+  <si>
+    <t>DESCRIPCION_INFRACION</t>
+  </si>
+  <si>
+    <t>FECHA_ENTRADA</t>
+  </si>
+  <si>
+    <t>FECHA_ASIGNACION</t>
+  </si>
+  <si>
+    <t>FECHA_ULTIMA_GESTION</t>
+  </si>
+  <si>
+    <t>RAZONSOCIAL</t>
+  </si>
+  <si>
+    <t>PRIMER_APELLIDO</t>
+  </si>
+  <si>
+    <t>SEGUNDO_APELLIDO</t>
+  </si>
+  <si>
+    <t>PRIMER_NOMBRE</t>
+  </si>
+  <si>
+    <t>SEGUNDO_NOMBRE</t>
+  </si>
+  <si>
+    <t>CAMPANAPORCLIENTE</t>
+  </si>
+  <si>
+    <t>SUBCAMPANAPORCLIENTE</t>
+  </si>
+  <si>
+    <t>USUARIOPORCLIENTE</t>
+  </si>
+  <si>
+    <t>CASACOBRANZAPORCLIENTE</t>
+  </si>
+  <si>
+    <t>FECHA_ULTIMA_FACT</t>
+  </si>
+  <si>
+    <t>MEJOR_RESPUESTA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +108,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -62,12 +139,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,124 +489,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>43</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>54</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>56</v>
-      </c>
-      <c r="D5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>54</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>34</v>
-      </c>
-      <c r="D7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>32</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pasar el contenido a un archivo de excel
</commit_message>
<xml_diff>
--- a/archivo.xlsx
+++ b/archivo.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Asignacion" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -491,7 +491,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>